<commit_message>
Atualização Dados SEAGRI e CEPEA
</commit_message>
<xml_diff>
--- a/Excel Preço local Barreiras.xlsx
+++ b/Excel Preço local Barreiras.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Pesquisa\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\MeusProjetos\Analise-Sincronia-SeriesTemporais-Soja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA51C694-D5E5-4094-9517-79820E49B286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCB197C-80D5-4687-A5D2-0EC2C2F3962B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2514"/>
+  <dimension ref="A1:E2611"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2598" workbookViewId="0">
+      <selection activeCell="B2610" sqref="B2610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -434,7 +434,7 @@
     <col min="2" max="2" width="16.109375" customWidth="1"/>
     <col min="3" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="18" width="8.6640625" customWidth="1"/>
+    <col min="6" max="14" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
@@ -20549,6 +20549,782 @@
       </c>
       <c r="B2514" s="3">
         <v>101.75</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2515" s="4">
+        <v>45338</v>
+      </c>
+      <c r="B2515" s="3">
+        <v>102.13</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2516" s="4">
+        <v>45341</v>
+      </c>
+      <c r="B2516" s="3">
+        <v>102.33</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2517" s="4">
+        <v>45342</v>
+      </c>
+      <c r="B2517" s="3">
+        <v>102.27</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2518" s="4">
+        <v>45343</v>
+      </c>
+      <c r="B2518" s="3">
+        <v>103.76</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2519" s="4">
+        <v>45344</v>
+      </c>
+      <c r="B2519" s="3">
+        <v>102.25</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2520" s="4">
+        <v>45345</v>
+      </c>
+      <c r="B2520" s="3">
+        <v>100.33</v>
+      </c>
+    </row>
+    <row r="2521" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2521" s="4">
+        <v>45348</v>
+      </c>
+      <c r="B2521" s="3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2522" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2522" s="4">
+        <v>45349</v>
+      </c>
+      <c r="B2522" s="3">
+        <v>108.38</v>
+      </c>
+    </row>
+    <row r="2523" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2523" s="4">
+        <v>45350</v>
+      </c>
+      <c r="B2523" s="3">
+        <v>101.63</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2524" s="4">
+        <v>45351</v>
+      </c>
+      <c r="B2524" s="3">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2525" s="4">
+        <v>45352</v>
+      </c>
+      <c r="B2525" s="3">
+        <v>99.75</v>
+      </c>
+    </row>
+    <row r="2526" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2526" s="4">
+        <v>45355</v>
+      </c>
+      <c r="B2526" s="3">
+        <v>100.38</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2527" s="4">
+        <v>45356</v>
+      </c>
+      <c r="B2527" s="3">
+        <v>101.38</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2528" s="4">
+        <v>45357</v>
+      </c>
+      <c r="B2528" s="3">
+        <v>101.63</v>
+      </c>
+    </row>
+    <row r="2529" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2529" s="4">
+        <v>45358</v>
+      </c>
+      <c r="B2529" s="3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2530" s="4">
+        <v>45359</v>
+      </c>
+      <c r="B2530" s="3">
+        <v>102.75</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2531" s="4">
+        <v>45362</v>
+      </c>
+      <c r="B2531" s="3">
+        <v>104.63</v>
+      </c>
+    </row>
+    <row r="2532" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2532" s="4">
+        <v>45363</v>
+      </c>
+      <c r="B2532" s="3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2533" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2533" s="4">
+        <v>45364</v>
+      </c>
+      <c r="B2533" s="3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2534" s="4">
+        <v>45365</v>
+      </c>
+      <c r="B2534" s="3">
+        <v>107.8</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2535" s="4">
+        <v>45366</v>
+      </c>
+      <c r="B2535" s="3">
+        <v>107.8</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2536" s="4">
+        <v>45369</v>
+      </c>
+      <c r="B2536" s="3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2537" s="4">
+        <v>45370</v>
+      </c>
+      <c r="B2537" s="3">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2538" s="4">
+        <v>45371</v>
+      </c>
+      <c r="B2538" s="3">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2539" s="4">
+        <v>45372</v>
+      </c>
+      <c r="B2539" s="3">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2540" s="4">
+        <v>45373</v>
+      </c>
+      <c r="B2540" s="3">
+        <v>107.75</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2541" s="4">
+        <v>45376</v>
+      </c>
+      <c r="B2541" s="3">
+        <v>107.88</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2542" s="4">
+        <v>45377</v>
+      </c>
+      <c r="B2542" s="3">
+        <v>108.25</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2543" s="4">
+        <v>45378</v>
+      </c>
+      <c r="B2543" s="3">
+        <v>107.88</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2544" s="4">
+        <v>45379</v>
+      </c>
+      <c r="B2544" s="3">
+        <v>106.63</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2545" s="4">
+        <v>45383</v>
+      </c>
+      <c r="B2545" s="3">
+        <v>106.63</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2546" s="4">
+        <v>45384</v>
+      </c>
+      <c r="B2546" s="3">
+        <v>107.88</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2547" s="4">
+        <v>45385</v>
+      </c>
+      <c r="B2547" s="3">
+        <v>108.75</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2548" s="4">
+        <v>45386</v>
+      </c>
+      <c r="B2548" s="3">
+        <v>108.63</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2549" s="4">
+        <v>45387</v>
+      </c>
+      <c r="B2549" s="3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2550" s="4">
+        <v>45390</v>
+      </c>
+      <c r="B2550" s="3">
+        <v>108.75</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2551" s="4">
+        <v>45391</v>
+      </c>
+      <c r="B2551" s="3">
+        <v>110.38</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2552" s="4">
+        <v>45392</v>
+      </c>
+      <c r="B2552" s="3">
+        <v>108.67</v>
+      </c>
+    </row>
+    <row r="2553" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2553" s="4">
+        <v>45393</v>
+      </c>
+      <c r="B2553" s="3">
+        <v>109.88</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2554" s="4">
+        <v>45394</v>
+      </c>
+      <c r="B2554" s="3">
+        <v>109.75</v>
+      </c>
+    </row>
+    <row r="2555" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2555" s="4">
+        <v>45397</v>
+      </c>
+      <c r="B2555" s="3">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2556" s="4">
+        <v>45398</v>
+      </c>
+      <c r="B2556" s="3">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2557" s="4">
+        <v>45399</v>
+      </c>
+      <c r="B2557" s="3">
+        <v>112.25</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2558" s="4">
+        <v>45400</v>
+      </c>
+      <c r="B2558" s="3">
+        <v>112.75</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2559" s="4">
+        <v>45401</v>
+      </c>
+      <c r="B2559" s="3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2560" s="4">
+        <v>45404</v>
+      </c>
+      <c r="B2560" s="3">
+        <v>111.25</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2561" s="4">
+        <v>45405</v>
+      </c>
+      <c r="B2561" s="3">
+        <v>111.25</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2562" s="4">
+        <v>45406</v>
+      </c>
+      <c r="B2562" s="3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2563" s="4">
+        <v>45407</v>
+      </c>
+      <c r="B2563" s="3">
+        <v>112.25</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2564" s="4">
+        <v>45408</v>
+      </c>
+      <c r="B2564" s="3">
+        <v>112.13</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2565" s="4">
+        <v>45411</v>
+      </c>
+      <c r="B2565" s="3">
+        <v>111.63</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2566" s="4">
+        <v>45412</v>
+      </c>
+      <c r="B2566" s="3">
+        <v>109.75</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2567" s="4">
+        <v>45414</v>
+      </c>
+      <c r="B2567" s="3">
+        <v>110.75</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2568" s="4">
+        <v>45415</v>
+      </c>
+      <c r="B2568" s="3">
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2569" s="4">
+        <v>45418</v>
+      </c>
+      <c r="B2569" s="3">
+        <v>111.38</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2570" s="4">
+        <v>45419</v>
+      </c>
+      <c r="B2570" s="3">
+        <v>111.38</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2571" s="4">
+        <v>45420</v>
+      </c>
+      <c r="B2571" s="3">
+        <v>115.5</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2572" s="4">
+        <v>45421</v>
+      </c>
+      <c r="B2572" s="3">
+        <v>115.38</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2573" s="4">
+        <v>45422</v>
+      </c>
+      <c r="B2573" s="3">
+        <v>114.88</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2574" s="4">
+        <v>45425</v>
+      </c>
+      <c r="B2574" s="3">
+        <v>114.75</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2575" s="4">
+        <v>45426</v>
+      </c>
+      <c r="B2575" s="3">
+        <v>115.63</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2576" s="4">
+        <v>45427</v>
+      </c>
+      <c r="B2576" s="3">
+        <v>115.63</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2577" s="4">
+        <v>45428</v>
+      </c>
+      <c r="B2577" s="3">
+        <v>115.63</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2578" s="4">
+        <v>45429</v>
+      </c>
+      <c r="B2578" s="3">
+        <v>115.63</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2579" s="4">
+        <v>45432</v>
+      </c>
+      <c r="B2579" s="3">
+        <v>115.63</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2580" s="4">
+        <v>45433</v>
+      </c>
+      <c r="B2580" s="3">
+        <v>115.63</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2581" s="4">
+        <v>45434</v>
+      </c>
+      <c r="B2581" s="3">
+        <v>117.25</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2582" s="4">
+        <v>45435</v>
+      </c>
+      <c r="B2582" s="3">
+        <v>117.5</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2583" s="4">
+        <v>45436</v>
+      </c>
+      <c r="B2583" s="3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2584" s="4">
+        <v>45439</v>
+      </c>
+      <c r="B2584" s="3">
+        <v>119.88</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2585" s="4">
+        <v>45440</v>
+      </c>
+      <c r="B2585" s="3">
+        <v>118.47</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2586" s="4">
+        <v>45441</v>
+      </c>
+      <c r="B2586" s="3">
+        <v>120.38</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2587" s="4">
+        <v>45446</v>
+      </c>
+      <c r="B2587" s="3">
+        <v>120.38</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2588" s="4">
+        <v>45447</v>
+      </c>
+      <c r="B2588" s="3">
+        <v>120.38</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2589" s="4">
+        <v>45448</v>
+      </c>
+      <c r="B2589" s="3">
+        <v>120.38</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2590" s="4">
+        <v>45449</v>
+      </c>
+      <c r="B2590" s="3">
+        <v>120.38</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2591" s="4">
+        <v>45450</v>
+      </c>
+      <c r="B2591" s="3">
+        <v>120.38</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2592" s="4">
+        <v>45451</v>
+      </c>
+      <c r="B2592" s="3">
+        <v>120.38</v>
+      </c>
+    </row>
+    <row r="2593" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2593" s="4">
+        <v>45453</v>
+      </c>
+      <c r="B2593" s="3">
+        <v>119.53</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2594" s="4">
+        <v>45454</v>
+      </c>
+      <c r="B2594" s="3">
+        <v>119.53</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2595" s="4">
+        <v>45455</v>
+      </c>
+      <c r="B2595" s="3">
+        <v>119.53</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2596" s="4">
+        <v>45456</v>
+      </c>
+      <c r="B2596" s="3">
+        <v>119.75</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2597" s="4">
+        <v>45457</v>
+      </c>
+      <c r="B2597" s="3">
+        <v>120.25</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2598" s="4">
+        <v>45460</v>
+      </c>
+      <c r="B2598" s="3">
+        <v>119.63</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2599" s="4">
+        <v>45460</v>
+      </c>
+      <c r="B2599" s="3">
+        <v>119.63</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2600" s="4">
+        <v>45461</v>
+      </c>
+      <c r="B2600" s="3">
+        <v>119.63</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2601" s="4">
+        <v>45462</v>
+      </c>
+      <c r="B2601" s="3">
+        <v>120.88</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2602" s="4">
+        <v>45463</v>
+      </c>
+      <c r="B2602" s="3">
+        <v>121.88</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2603" s="4">
+        <v>45468</v>
+      </c>
+      <c r="B2603" s="3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2604" s="4">
+        <v>45469</v>
+      </c>
+      <c r="B2604" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2605" s="4">
+        <v>45470</v>
+      </c>
+      <c r="B2605" s="3">
+        <v>121.38</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2606" s="4">
+        <v>45471</v>
+      </c>
+      <c r="B2606" s="3">
+        <v>120.75</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2607" s="4">
+        <v>45474</v>
+      </c>
+      <c r="B2607" s="3">
+        <v>121.5</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2608" s="4">
+        <v>45476</v>
+      </c>
+      <c r="B2608" s="3">
+        <v>121.38</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2609" s="4">
+        <v>45477</v>
+      </c>
+      <c r="B2609" s="3">
+        <v>122.5</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2610" s="4">
+        <v>45478</v>
+      </c>
+      <c r="B2610" s="3">
+        <v>122.5</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2611" s="4">
+        <v>45481</v>
+      </c>
+      <c r="B2611" s="3">
+        <v>122.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>